<commit_message>
OpenDEP v1.4.0 Added the live image aquisition module. For now it works only with DSRL. Enjoy!
</commit_message>
<xml_diff>
--- a/tests/Data.xlsx
+++ b/tests/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef108f43608dd4eb/Programming/Python/OpenDEP/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{FDE7A924-E319-4547-A276-50874F653EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96A9AD3E-8939-4E9C-951B-2AA08A3DB375}"/>
+  <xr:revisionPtr revIDLastSave="202" documentId="8_{FDE7A924-E319-4547-A276-50874F653EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{759BDAC9-94D9-47A7-B732-E31777F89278}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{29490AAE-8766-4DCC-993E-81AB7C629939}"/>
   </bookViews>
@@ -65,22 +65,22 @@
     <t>Color</t>
   </si>
   <si>
-    <t>50, 50, 50</t>
-  </si>
-  <si>
-    <t>125, 125, 125</t>
-  </si>
-  <si>
     <t>MSC</t>
   </si>
   <si>
-    <t>200, 200, 200</t>
+    <t>192, 0, 0</t>
+  </si>
+  <si>
+    <t>46, 117, 181</t>
+  </si>
+  <si>
+    <t>201, 196, 0</t>
+  </si>
+  <si>
+    <t>Week 2</t>
   </si>
   <si>
     <t>Week 4</t>
-  </si>
-  <si>
-    <t>Week 2</t>
   </si>
 </sst>
 </file>
@@ -105,19 +105,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF323232"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7D7D7D"/>
+        <fgColor rgb="FFC9C400"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC8C8C8"/>
+        <fgColor rgb="FF2F75B5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -170,6 +170,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC9C400"/>
+      <color rgb="FF2F75B5"/>
+      <color rgb="FFBFB101"/>
+      <color rgb="FFC65911"/>
       <color rgb="FFC8C8C8"/>
       <color rgb="FFAFAFAF"/>
       <color rgb="FF7D7D7D"/>
@@ -488,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F99F61AD-899A-4762-9A82-7DDBC46ED6D5}">
   <dimension ref="A2:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,13 +512,13 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -522,13 +526,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -593,19 +597,19 @@
         <v>10000</v>
       </c>
       <c r="E8">
-        <v>-0.35309502838341422</v>
+        <v>-0.48546086796777138</v>
       </c>
       <c r="F8">
-        <v>0.18725864771021911</v>
+        <v>0.18746840117491509</v>
       </c>
       <c r="G8">
         <v>10000</v>
       </c>
       <c r="H8">
-        <v>-0.34089891112253179</v>
+        <v>-0.63614108420724969</v>
       </c>
       <c r="I8">
-        <v>0.2025793918811172</v>
+        <v>0.16993870483820531</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -622,19 +626,19 @@
         <v>15473.270035805101</v>
       </c>
       <c r="E9">
-        <v>-0.34050766729940118</v>
+        <v>-0.46275766771530069</v>
       </c>
       <c r="F9">
-        <v>0.15782422403172511</v>
+        <v>0.15363764879060521</v>
       </c>
       <c r="G9">
         <v>15473.270035805101</v>
       </c>
       <c r="H9">
-        <v>-0.37368768520962942</v>
+        <v>-0.58092014091749988</v>
       </c>
       <c r="I9">
-        <v>0.23988258842798671</v>
+        <v>0.10850770325221649</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -651,19 +655,19 @@
         <v>23942.208560094499</v>
       </c>
       <c r="E10">
-        <v>-0.24419814592708519</v>
+        <v>-0.46833474300334899</v>
       </c>
       <c r="F10">
-        <v>0.14081263813417211</v>
+        <v>0.1197297490182557</v>
       </c>
       <c r="G10">
         <v>23942.208560094499</v>
       </c>
       <c r="H10">
-        <v>-0.33258844693785378</v>
+        <v>-0.58420095682101469</v>
       </c>
       <c r="I10">
-        <v>0.23536180488682851</v>
+        <v>0.1065915558549448</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -680,19 +684,19 @@
         <v>37046.425830390603</v>
       </c>
       <c r="E11">
-        <v>-5.1857126013983297E-2</v>
+        <v>-0.3457915731397071</v>
       </c>
       <c r="F11">
-        <v>0.1400178964819791</v>
+        <v>0.1305695272008498</v>
       </c>
       <c r="G11">
         <v>37046.425830390603</v>
       </c>
       <c r="H11">
-        <v>-0.1376794678155516</v>
+        <v>-0.48944175066803358</v>
       </c>
       <c r="I11">
-        <v>0.21770260335399971</v>
+        <v>0.126894092428678</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -709,19 +713,19 @@
         <v>57322.935073505992</v>
       </c>
       <c r="E12">
-        <v>4.8017913521575938E-2</v>
+        <v>-0.15802938796665411</v>
       </c>
       <c r="F12">
-        <v>0.11539441192248499</v>
+        <v>0.12813926051454899</v>
       </c>
       <c r="G12">
         <v>57322.935073505992</v>
       </c>
       <c r="H12">
-        <v>-6.7061666054081231E-2</v>
+        <v>-0.32816054254315402</v>
       </c>
       <c r="I12">
-        <v>0.2135826005308179</v>
+        <v>0.14138396349778609</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -738,19 +742,19 @@
         <v>88697.325363728305</v>
       </c>
       <c r="E13">
-        <v>0.15459741912451061</v>
+        <v>-4.9963114790471393E-2</v>
       </c>
       <c r="F13">
-        <v>0.12955804533973089</v>
+        <v>0.14892305331357589</v>
       </c>
       <c r="G13">
         <v>88697.325363728305</v>
       </c>
       <c r="H13">
-        <v>8.66231435103673E-4</v>
+        <v>-0.32911663645696082</v>
       </c>
       <c r="I13">
-        <v>0.18570862901566099</v>
+        <v>0.17032447952602911</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -767,19 +771,19 @@
         <v>137243.766680664</v>
       </c>
       <c r="E14">
-        <v>0.32540044732162748</v>
+        <v>0.125694869768432</v>
       </c>
       <c r="F14">
-        <v>0.12152920605330921</v>
+        <v>0.1475112527471121</v>
       </c>
       <c r="G14">
         <v>137243.766680664</v>
       </c>
       <c r="H14">
-        <v>0.1538835237626823</v>
+        <v>-0.2245416232779831</v>
       </c>
       <c r="I14">
-        <v>0.22061713484540341</v>
+        <v>0.1878003095820226</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -796,19 +800,19 @@
         <v>212360.986258094</v>
       </c>
       <c r="E15">
-        <v>0.4183977132539799</v>
+        <v>0.24737001840820561</v>
       </c>
       <c r="F15">
-        <v>9.7082082175892592E-2</v>
+        <v>0.12507367236285549</v>
       </c>
       <c r="G15">
         <v>212360.986258094</v>
       </c>
       <c r="H15">
-        <v>0.25800107810619177</v>
+        <v>-0.13106571087381491</v>
       </c>
       <c r="I15">
-        <v>0.23977573731503871</v>
+        <v>0.20256663164473121</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -825,19 +829,19 @@
         <v>328591.88854413899</v>
       </c>
       <c r="E16">
-        <v>0.44174898924461908</v>
+        <v>0.32905731008005668</v>
       </c>
       <c r="F16">
-        <v>0.1043803248463885</v>
+        <v>0.13110946208082111</v>
       </c>
       <c r="G16">
         <v>328591.88854413899</v>
       </c>
       <c r="H16">
-        <v>0.33336129293894862</v>
+        <v>1.9401026315457068E-2</v>
       </c>
       <c r="I16">
-        <v>0.16784796028573329</v>
+        <v>0.22894394933505341</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -854,19 +858,19 @@
         <v>508439.10230186413</v>
       </c>
       <c r="E17">
-        <v>0.45446197677549161</v>
+        <v>0.36249149708094502</v>
       </c>
       <c r="F17">
-        <v>0.13695456425230421</v>
+        <v>9.6617525817777661E-2</v>
       </c>
       <c r="G17">
         <v>508439.10230186413</v>
       </c>
       <c r="H17">
-        <v>0.4259303729546578</v>
+        <v>5.8406048065446733E-2</v>
       </c>
       <c r="I17">
-        <v>0.26038343315836748</v>
+        <v>0.19947635904147201</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -883,19 +887,19 @@
         <v>786721.55266790802</v>
       </c>
       <c r="E18">
-        <v>0.51801115253805696</v>
+        <v>0.44185239677860899</v>
       </c>
       <c r="F18">
-        <v>0.1002322170559906</v>
+        <v>0.10573133907346841</v>
       </c>
       <c r="G18">
         <v>786721.55266790802</v>
       </c>
       <c r="H18">
-        <v>0.45012085057075929</v>
+        <v>0.18888910377586229</v>
       </c>
       <c r="I18">
-        <v>0.1067383184292498</v>
+        <v>0.20931812510398681</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -912,19 +916,19 @@
         <v>1217315.50274184</v>
       </c>
       <c r="E19">
-        <v>0.67426441351182431</v>
+        <v>0.61045978921674815</v>
       </c>
       <c r="F19">
-        <v>0.1147347494384542</v>
+        <v>0.1187975587422307</v>
       </c>
       <c r="G19">
         <v>1217315.50274184</v>
       </c>
       <c r="H19">
-        <v>0.58401406602043893</v>
+        <v>0.34734150658736013</v>
       </c>
       <c r="I19">
-        <v>0.19818276357642151</v>
+        <v>0.2124636996169833</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -941,19 +945,19 @@
         <v>1883585.14926964</v>
       </c>
       <c r="E20">
-        <v>0.72947750463139993</v>
+        <v>0.68881400757782685</v>
       </c>
       <c r="F20">
-        <v>0.1238405653689502</v>
+        <v>0.12574584984886461</v>
       </c>
       <c r="G20">
         <v>1883585.14926964</v>
       </c>
       <c r="H20">
-        <v>0.63119769004947479</v>
+        <v>0.44854443221939672</v>
       </c>
       <c r="I20">
-        <v>0.16183447544516191</v>
+        <v>0.1815958943207383</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -970,19 +974,19 @@
         <v>2914522.1650081398</v>
       </c>
       <c r="E21">
-        <v>0.67961362800685698</v>
+        <v>0.69654406430585936</v>
       </c>
       <c r="F21">
-        <v>0.11256475342488841</v>
+        <v>0.1204988726650472</v>
       </c>
       <c r="G21">
         <v>2914522.1650081398</v>
       </c>
       <c r="H21">
-        <v>0.6675004153018248</v>
+        <v>0.47317913322620969</v>
       </c>
       <c r="I21">
-        <v>0.1422072426287373</v>
+        <v>0.22342627318221239</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -999,19 +1003,19 @@
         <v>4509718.8484510398</v>
       </c>
       <c r="E22">
-        <v>0.57158070578064479</v>
+        <v>0.55893295908253027</v>
       </c>
       <c r="F22">
-        <v>0.1390151102554972</v>
+        <v>0.14919944655093631</v>
       </c>
       <c r="G22">
         <v>4509718.8484510398</v>
       </c>
       <c r="H22">
-        <v>0.59125955737145997</v>
+        <v>0.44400092533571978</v>
       </c>
       <c r="I22">
-        <v>0.19314268500897969</v>
+        <v>0.20587830967869639</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -1028,19 +1032,19 @@
         <v>6978009.7527643014</v>
       </c>
       <c r="E23">
-        <v>0.55906668898399581</v>
+        <v>0.58556987886072753</v>
       </c>
       <c r="F23">
-        <v>0.12811143341752571</v>
+        <v>0.1477458350178717</v>
       </c>
       <c r="G23">
         <v>6978009.7527643014</v>
       </c>
       <c r="H23">
-        <v>0.66037844862333972</v>
+        <v>0.4829755009194428</v>
       </c>
       <c r="I23">
-        <v>0.1803866483621632</v>
+        <v>0.20979583464064611</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1057,19 +1061,19 @@
         <v>10797262.921700399</v>
       </c>
       <c r="E24">
-        <v>0.61652209165871441</v>
+        <v>0.60024550809858213</v>
       </c>
       <c r="F24">
-        <v>0.1230098902276679</v>
+        <v>0.115695652777702</v>
       </c>
       <c r="G24">
         <v>10797262.921700399</v>
       </c>
       <c r="H24">
-        <v>0.65662724223563129</v>
+        <v>0.49437602358120308</v>
       </c>
       <c r="I24">
-        <v>0.19324031990369761</v>
+        <v>0.21983088433863149</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1086,19 +1090,19 @@
         <v>16706896.483505599</v>
       </c>
       <c r="E25">
-        <v>0.43915993208871662</v>
+        <v>0.48430733951775151</v>
       </c>
       <c r="F25">
-        <v>0.1152949113512462</v>
+        <v>8.9921273484578429E-2</v>
       </c>
       <c r="G25">
         <v>16706896.483505599</v>
       </c>
       <c r="H25">
-        <v>0.46510411108430971</v>
+        <v>0.39519775368973331</v>
       </c>
       <c r="I25">
-        <v>0.15765361732429381</v>
+        <v>0.15920971354636801</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1115,19 +1119,19 @@
         <v>25851032.074952502</v>
       </c>
       <c r="E26">
-        <v>0.21268190794884331</v>
+        <v>0.25485474472495168</v>
       </c>
       <c r="F26">
-        <v>8.4695959166774859E-2</v>
+        <v>0.112773092203344</v>
       </c>
       <c r="G26">
         <v>25851032.074952502</v>
       </c>
       <c r="H26">
-        <v>0.20082175459270171</v>
+        <v>0.17441887422429631</v>
       </c>
       <c r="I26">
-        <v>0.1625964114732828</v>
+        <v>9.5620494474861081E-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1144,19 +1148,19 @@
         <v>40000000</v>
       </c>
       <c r="E27">
-        <v>9.5164965562693854E-2</v>
+        <v>8.8770039175045029E-2</v>
       </c>
       <c r="F27">
-        <v>9.9945067250716862E-2</v>
+        <v>0.13565462164898931</v>
       </c>
       <c r="G27">
         <v>40000000</v>
       </c>
       <c r="H27">
-        <v>0.1336097169628955</v>
+        <v>0.15123762536673829</v>
       </c>
       <c r="I27">
-        <v>0.26388420012258479</v>
+        <v>0.1769990444366098</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1203,13 +1207,13 @@
         <v>7000.0000000000018</v>
       </c>
       <c r="E31">
-        <v>-0.30638343348002051</v>
+        <v>-0.4119711805800243</v>
       </c>
       <c r="G31">
         <v>7000.0000000000018</v>
       </c>
       <c r="H31">
-        <v>-0.29597108046638138</v>
+        <v>-0.46729636463375812</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1223,13 +1227,13 @@
         <v>8421.01482776388</v>
       </c>
       <c r="E32">
-        <v>-0.30312785687135191</v>
+        <v>-0.41073107957746369</v>
       </c>
       <c r="G32">
         <v>8421.01482776388</v>
       </c>
       <c r="H32">
-        <v>-0.29429891644778983</v>
+        <v>-0.46705923887563128</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1243,13 +1247,13 @@
         <v>10130.498675631299</v>
       </c>
       <c r="E33">
-        <v>-0.29847268222111978</v>
+        <v>-0.40894317884019138</v>
       </c>
       <c r="G33">
         <v>10130.498675631299</v>
       </c>
       <c r="H33">
-        <v>-0.29191683294388998</v>
+        <v>-0.4667164648335787</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1263,13 +1267,13 @@
         <v>12187.01136573338</v>
       </c>
       <c r="E34">
-        <v>-0.29185031409478679</v>
+        <v>-0.40636981130010219</v>
       </c>
       <c r="G34">
         <v>12187.01136573338</v>
       </c>
       <c r="H34">
-        <v>-0.28854508305959969</v>
+        <v>-0.46622122797582971</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1283,13 +1287,13 @@
         <v>14661.00048813825</v>
       </c>
       <c r="E35">
-        <v>-0.28249693332398668</v>
+        <v>-0.40267480001820888</v>
       </c>
       <c r="G35">
         <v>14661.00048813825</v>
       </c>
       <c r="H35">
-        <v>-0.28381349718193372</v>
+        <v>-0.46550624659862339</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1303,13 +1307,13 @@
         <v>17637.21464292366</v>
       </c>
       <c r="E36">
-        <v>-0.2694168282712599</v>
+        <v>-0.39738746674911501</v>
       </c>
       <c r="G36">
         <v>17637.21464292366</v>
       </c>
       <c r="H36">
-        <v>-0.27724827670350632</v>
+        <v>-0.46447512222928838</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1323,13 +1327,13 @@
         <v>21217.60657550209</v>
       </c>
       <c r="E37">
-        <v>-0.25137011149605187</v>
+        <v>-0.38985851169265268</v>
       </c>
       <c r="G37">
         <v>21217.60657550209</v>
       </c>
       <c r="H37">
-        <v>-0.26826777226521747</v>
+        <v>-0.46299035386969711</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1343,13 +1347,13 @@
         <v>25524.825654566212</v>
       </c>
       <c r="E38">
-        <v>-0.22691292628096471</v>
+        <v>-0.37921127576793212</v>
       </c>
       <c r="G38">
         <v>25524.825654566212</v>
       </c>
       <c r="H38">
-        <v>-0.25619205527702849</v>
+        <v>-0.46085706901882217</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1363,13 +1367,13 @@
         <v>30706.419330455701</v>
       </c>
       <c r="E39">
-        <v>-0.19452731270363269</v>
+        <v>-0.36429860246961859</v>
       </c>
       <c r="G39">
         <v>30706.419330455701</v>
       </c>
       <c r="H39">
-        <v>-0.2402667852344402</v>
+        <v>-0.45780162588551909</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1383,13 +1387,13 @@
         <v>36939.887498471828</v>
       </c>
       <c r="E40">
-        <v>-0.1528717066581137</v>
+        <v>-0.34368680228951598</v>
       </c>
       <c r="G40">
         <v>36939.887498471828</v>
       </c>
       <c r="H40">
-        <v>-0.21969607700921601</v>
+        <v>-0.453444832125802</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1403,13 +1407,13 @@
         <v>44438.762908651537</v>
       </c>
       <c r="E41">
-        <v>-0.1011489669910441</v>
+        <v>-0.31570318241004502</v>
       </c>
       <c r="G41">
         <v>44438.762908651537</v>
       </c>
       <c r="H41">
-        <v>-0.193680161331827</v>
+        <v>-0.44727108919945319</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1423,13 +1427,13 @@
         <v>53459.925911605547</v>
       </c>
       <c r="E42">
-        <v>-3.9522040175728211E-2</v>
+        <v>-0.27859534173404948</v>
       </c>
       <c r="G42">
         <v>53459.925911605547</v>
       </c>
       <c r="H42">
-        <v>-0.16146788387555269</v>
+        <v>-0.43859797031003639</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1443,13 +1447,13 @@
         <v>64312.404113255521</v>
       </c>
       <c r="E43">
-        <v>3.0571204848188038E-2</v>
+        <v>-0.23084223833990211</v>
       </c>
       <c r="G43">
         <v>64312.404113255521</v>
       </c>
       <c r="H43">
-        <v>-0.1224494610183938</v>
+        <v>-0.42655610164091762</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1463,13 +1467,13 @@
         <v>77367.958378123905</v>
       </c>
       <c r="E44">
-        <v>0.1063859867215063</v>
+        <v>-0.17160688276215511</v>
       </c>
       <c r="G44">
         <v>77367.958378123905</v>
       </c>
       <c r="H44">
-        <v>-7.6305694974622015E-2</v>
+        <v>-0.41009617866754239</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,13 +1487,13 @@
         <v>93073.817813714471</v>
       </c>
       <c r="E45">
-        <v>0.18422510559380931</v>
+        <v>-0.10122497297843321</v>
       </c>
       <c r="G45">
         <v>93073.817813714471</v>
       </c>
       <c r="H45">
-        <v>-2.3191822641422659E-2</v>
+        <v>-0.38804513933405799</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1503,13 +1507,13 @@
         <v>111967.99998369761</v>
       </c>
       <c r="E46">
-        <v>0.2600980599262529</v>
+        <v>-2.153135645661608E-2</v>
       </c>
       <c r="G46">
         <v>111967.99998369761</v>
       </c>
       <c r="H46">
-        <v>3.6102714875844599E-2</v>
+        <v>-0.35922956197730282</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1523,13 +1527,13 @@
         <v>134697.7411568262</v>
       </c>
       <c r="E47">
-        <v>0.3304397010074368</v>
+        <v>6.4173591321860068E-2</v>
       </c>
       <c r="G47">
         <v>134697.7411568262</v>
       </c>
       <c r="H47">
-        <v>0.1000865871512434</v>
+        <v>-0.32266318460413901</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1543,13 +1547,13 @@
         <v>162041.6679354191</v>
       </c>
       <c r="E48">
-        <v>0.39264150336178882</v>
+        <v>0.1515819949059834</v>
       </c>
       <c r="G48">
         <v>162041.6679354191</v>
       </c>
       <c r="H48">
-        <v>0.16664192180753989</v>
+        <v>-0.27775952941324389</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1563,13 +1567,13 @@
         <v>194936.4697713936</v>
       </c>
       <c r="E49">
-        <v>0.44528399408814617</v>
+        <v>0.23613665230334921</v>
       </c>
       <c r="G49">
         <v>194936.4697713936</v>
       </c>
       <c r="H49">
-        <v>0.23325714682569521</v>
+        <v>-0.22450362907786139</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1583,13 +1587,13 @@
         <v>234508.98605955049</v>
       </c>
       <c r="E50">
-        <v>0.48809122607080369</v>
+        <v>0.31384371771148117</v>
       </c>
       <c r="G50">
         <v>234508.98605955049</v>
       </c>
       <c r="H50">
-        <v>0.29737746945935373</v>
+        <v>-0.16352967732641821</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1603,13 +1607,13 @@
         <v>282114.80697876401</v>
       </c>
       <c r="E51">
-        <v>0.5216892598844376</v>
+        <v>0.38188830466486851</v>
       </c>
       <c r="G51">
         <v>282114.80697876401</v>
       </c>
       <c r="H51">
-        <v>0.35677740425497201</v>
+        <v>-9.6101293555379871E-2</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1623,13 +1627,13 @@
         <v>339384.7103857022</v>
       </c>
       <c r="E52">
-        <v>0.5472698287560972</v>
+        <v>0.43889265386633319</v>
       </c>
       <c r="G52">
         <v>339384.7103857022</v>
       </c>
       <c r="H52">
-        <v>0.40983856809443669</v>
+        <v>-2.4030317589119152E-2</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1643,13 +1647,13 @@
         <v>408280.52549633622</v>
       </c>
       <c r="E53">
-        <v>0.56625950942598013</v>
+        <v>0.48480534679474641</v>
       </c>
       <c r="G53">
         <v>408280.52549633622</v>
       </c>
       <c r="H53">
-        <v>0.45565666805649369</v>
+        <v>5.0436598126739021E-2</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1663,13 +1667,13 @@
         <v>491162.33701312513</v>
       </c>
       <c r="E54">
-        <v>0.58006647943728129</v>
+        <v>0.52054488718119374</v>
       </c>
       <c r="G54">
         <v>491162.33701312513</v>
       </c>
       <c r="H54">
-        <v>0.49398659515514459</v>
+        <v>0.12476368098531899</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1683,13 +1687,13 @@
         <v>590869.33183238353</v>
       </c>
       <c r="E55">
-        <v>0.58993011115023275</v>
+        <v>0.54756986255710927</v>
       </c>
       <c r="G55">
         <v>590869.33183238353</v>
       </c>
       <c r="H55">
-        <v>0.52510004177935887</v>
+        <v>0.1963178798310222</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1703,13 +1707,13 @@
         <v>710817.05780449091</v>
       </c>
       <c r="E56">
-        <v>0.59685949642453628</v>
+        <v>0.56750776372733247</v>
       </c>
       <c r="G56">
         <v>710817.05780449091</v>
       </c>
       <c r="H56">
-        <v>0.5496284433855857</v>
+        <v>0.26261489947578559</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1723,13 +1727,13 @@
         <v>855114.42622844467</v>
       </c>
       <c r="E57">
-        <v>0.60163019892049285</v>
+        <v>0.58190097112580974</v>
       </c>
       <c r="G57">
         <v>855114.42622844467</v>
       </c>
       <c r="H57">
-        <v>0.56841993689902226</v>
+        <v>0.32160526099949199</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1743,13 +1747,13 @@
         <v>1028704.46610065</v>
       </c>
       <c r="E58">
-        <v>0.60480996885939986</v>
+        <v>0.59206995386229055</v>
       </c>
       <c r="G58">
         <v>1028704.46610065</v>
       </c>
       <c r="H58">
-        <v>0.58241028848024801</v>
+        <v>0.37194042183099058</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -1763,13 +1767,13 @@
         <v>1237533.6517743559</v>
       </c>
       <c r="E59">
-        <v>0.60679310272751585</v>
+        <v>0.59906454825017907</v>
       </c>
       <c r="G59">
         <v>1237533.6517743559</v>
       </c>
       <c r="H59">
-        <v>0.59251041279374861</v>
+        <v>0.41311837719377392</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -1783,13 +1787,13 @@
         <v>1488755.604492662</v>
       </c>
       <c r="E60">
-        <v>0.60783204015864711</v>
+        <v>0.60366802602006098</v>
       </c>
       <c r="G60">
         <v>1488755.604492662</v>
       </c>
       <c r="H60">
-        <v>0.59952131088900207</v>
+        <v>0.44543368565598979</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -1803,13 +1807,13 @@
         <v>1790976.145764187</v>
       </c>
       <c r="E61">
-        <v>0.60806089305868216</v>
+        <v>0.60642476190589023</v>
       </c>
       <c r="G61">
         <v>1790976.145764187</v>
       </c>
       <c r="H61">
-        <v>0.60408293987439499</v>
+        <v>0.46975036512039259</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -1823,13 +1827,13 @@
         <v>2154548.0970930881</v>
       </c>
       <c r="E62">
-        <v>0.60750890000937907</v>
+        <v>0.60767200946889477</v>
       </c>
       <c r="G62">
         <v>2154548.0970930881</v>
       </c>
       <c r="H62">
-        <v>0.60665241297916916</v>
+        <v>0.48719754192285852</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -1843,13 +1847,13 @@
         <v>2591925.9246787629</v>
       </c>
       <c r="E63">
-        <v>0.60610318240312466</v>
+        <v>0.60756474332034638</v>
       </c>
       <c r="G63">
         <v>2591925.9246787629</v>
       </c>
       <c r="H63">
-        <v>0.60749966393402088</v>
+        <v>0.49889392186004328</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -1863,13 +1867,13 @@
         <v>3118092.3777407799</v>
       </c>
       <c r="E64">
-        <v>0.60366055256120443</v>
+        <v>0.60608818809312548</v>
       </c>
       <c r="G64">
         <v>3118092.3777407799</v>
       </c>
       <c r="H64">
-        <v>0.60670807432634744</v>
+        <v>0.50575615116847283</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -1883,13 +1887,13 @@
         <v>3751071.735327519</v>
       </c>
       <c r="E65">
-        <v>0.59986822825342523</v>
+        <v>0.60305592971633648</v>
       </c>
       <c r="G65">
         <v>3751071.735327519</v>
       </c>
       <c r="H65">
-        <v>0.604170840781179</v>
+        <v>0.50839230027645033</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -1903,13 +1907,13 @@
         <v>4512547.2433141554</v>
       </c>
       <c r="E66">
-        <v>0.59425384469094078</v>
+        <v>0.59809357598206003</v>
       </c>
       <c r="G66">
         <v>4512547.2433141554</v>
       </c>
       <c r="H66">
-        <v>0.59957827341168046</v>
+        <v>0.50705544818202786</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -1923,13 +1927,13 @@
         <v>5428603.8924190737</v>
       </c>
       <c r="E67">
-        <v>0.58614701435008243</v>
+        <v>0.59061025503465514</v>
       </c>
       <c r="G67">
         <v>5428603.8924190737</v>
       </c>
       <c r="H67">
-        <v>0.59239601533340558</v>
+        <v>0.50163235689940533</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -1943,13 +1947,13 @@
         <v>6530621.9817311028</v>
       </c>
       <c r="E68">
-        <v>0.57463914045663755</v>
+        <v>0.57976448810592596</v>
       </c>
       <c r="G68">
         <v>6530621.9817311028</v>
       </c>
       <c r="H68">
-        <v>0.58184030511461005</v>
+        <v>0.49165601759650462</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -1963,13 +1967,13 @@
         <v>7856352.0775254937</v>
       </c>
       <c r="E69">
-        <v>0.55855681730502971</v>
+        <v>0.56443900816582493</v>
       </c>
       <c r="G69">
         <v>7856352.0775254937</v>
       </c>
       <c r="H69">
-        <v>0.56686552342114405</v>
+        <v>0.47634858495488341</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -1983,13 +1987,13 @@
         <v>9451208.1909965314</v>
       </c>
       <c r="E70">
-        <v>0.53647787300762295</v>
+        <v>0.54325223396780264</v>
       </c>
       <c r="G70">
         <v>9451208.1909965314</v>
       </c>
       <c r="H70">
-        <v>0.54619217241447748</v>
+        <v>0.45471659042295731</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2003,13 +2007,13 @@
         <v>11369823.47380932</v>
       </c>
       <c r="E71">
-        <v>0.50683536759314463</v>
+        <v>0.51465061314579141</v>
       </c>
       <c r="G71">
         <v>11369823.47380932</v>
       </c>
       <c r="H71">
-        <v>0.51841704531954624</v>
+        <v>0.42572631726812371</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -2023,13 +2027,13 @@
         <v>13677921.723143719</v>
       </c>
       <c r="E72">
-        <v>0.46816247988946352</v>
+        <v>0.47713611607833939</v>
       </c>
       <c r="G72">
         <v>13677921.723143719</v>
       </c>
       <c r="H72">
-        <v>0.48225005789888192</v>
+        <v>0.38857428586770898</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -2043,13 +2047,13 @@
         <v>16454568.806226701</v>
       </c>
       <c r="E73">
-        <v>0.41950663457772941</v>
+        <v>0.42966415409420311</v>
       </c>
       <c r="G73">
         <v>16454568.806226701</v>
       </c>
       <c r="H73">
-        <v>0.43689218057563689</v>
+        <v>0.34302890141356213</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -2063,13 +2067,13 @@
         <v>19794881.128813758</v>
       </c>
       <c r="E74">
-        <v>0.36095825018211308</v>
+        <v>0.37217060534993079</v>
       </c>
       <c r="G74">
         <v>19794881.128813758</v>
       </c>
       <c r="H74">
-        <v>0.3824873123199391</v>
+        <v>0.28976049808453452</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -2083,13 +2087,13 @@
         <v>23813283.92850915</v>
       </c>
       <c r="E75">
-        <v>0.29410638444995602</v>
+        <v>0.30605322643395361</v>
       </c>
       <c r="G75">
         <v>23813283.92850915</v>
       </c>
       <c r="H75">
-        <v>0.32046894751360561</v>
+        <v>0.23052568324620731</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2103,13 +2107,13 @@
         <v>28647431.008532401</v>
       </c>
       <c r="E76">
-        <v>0.22213737391973629</v>
+        <v>0.23432305896089869</v>
       </c>
       <c r="G76">
         <v>28647431.008532401</v>
       </c>
       <c r="H76">
-        <v>0.25357081066546588</v>
+        <v>0.16807341926812461</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -2123,13 +2127,13 @@
         <v>34462920.18574208</v>
       </c>
       <c r="E77">
-        <v>0.1493703913506336</v>
+        <v>0.16119972161325419</v>
       </c>
       <c r="G77">
         <v>34462920.18574208</v>
       </c>
       <c r="H77">
-        <v>0.1853838128530263</v>
+        <v>0.10573076201485659</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -2143,13 +2147,13 @@
         <v>41458965.984596729</v>
       </c>
       <c r="E78">
-        <v>8.0312325291218359E-2</v>
+        <v>9.1205140384262681E-2</v>
       </c>
       <c r="G78">
         <v>41458965.984596729</v>
       </c>
       <c r="H78">
-        <v>0.1195942084146938</v>
+        <v>4.6780421277632933E-2</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -2163,13 +2167,13 @@
         <v>49875223.900006764</v>
       </c>
       <c r="E79">
-        <v>1.8626517520461731E-2</v>
+        <v>2.8131809853440371E-2</v>
       </c>
       <c r="G79">
         <v>49875223.900006764</v>
       </c>
       <c r="H79">
-        <v>5.9232067412318477E-2</v>
+        <v>-6.1422595322078131E-3</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2183,13 +2187,13 @@
         <v>60000000.000000022</v>
       </c>
       <c r="E80" s="2">
-        <v>-3.3529023433842467E-2</v>
+        <v>-2.5659887741122909E-2</v>
       </c>
       <c r="G80">
         <v>60000000.000000022</v>
       </c>
       <c r="H80" s="2">
-        <v>6.2253221579963531E-3</v>
+        <v>-5.142198654111059E-2</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
OpenDEP Compute v1.0.2 Added the option to compute OpenDEP Population whitout any need of bkg images obtained before DEP exposure. Enjoy!
</commit_message>
<xml_diff>
--- a/tests/Data.xlsx
+++ b/tests/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef108f43608dd4eb/Programming/Python/OpenDEP/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="237" documentId="8_{FDE7A924-E319-4547-A276-50874F653EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BE2DD74-B0DD-4905-B8A2-959917465123}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{FDE7A924-E319-4547-A276-50874F653EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AB949D8-6AB2-41A2-AA78-21A7C42B989E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{29490AAE-8766-4DCC-993E-81AB7C629939}"/>
   </bookViews>
@@ -181,9 +181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,7 +221,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -327,7 +327,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -469,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -480,7 +480,7 @@
   <dimension ref="A2:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,19 +552,19 @@
         <v>5000</v>
       </c>
       <c r="B8">
-        <v>-0.88146875085560961</v>
+        <v>-0.55684185833150623</v>
       </c>
       <c r="C8">
-        <v>4.2280511441687152E-2</v>
+        <v>0.12782251426079561</v>
       </c>
       <c r="D8">
         <v>5000</v>
       </c>
       <c r="E8">
-        <v>-0.27029755419749929</v>
+        <v>-0.48696027863483571</v>
       </c>
       <c r="F8">
-        <v>0.26365844031251068</v>
+        <v>1.8922736057858887E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -572,19 +572,19 @@
         <v>7500</v>
       </c>
       <c r="B9">
-        <v>-0.50607320172537817</v>
+        <v>-0.68728672810513869</v>
       </c>
       <c r="C9">
-        <v>0.2770834921308748</v>
+        <v>9.3611532982719695E-2</v>
       </c>
       <c r="D9">
         <v>7500</v>
       </c>
       <c r="E9">
-        <v>-0.29512395900395189</v>
+        <v>-0.60034963746509717</v>
       </c>
       <c r="F9">
-        <v>0.27036611557747064</v>
+        <v>2.4052995837006329E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -592,19 +592,19 @@
         <v>10000</v>
       </c>
       <c r="B10">
-        <v>-0.37815288743515119</v>
+        <v>-0.57041438864915051</v>
       </c>
       <c r="C10">
-        <v>2.3436501321182635E-3</v>
+        <v>0.11908190729207413</v>
       </c>
       <c r="D10">
         <v>10000</v>
       </c>
       <c r="E10">
-        <v>-0.2821905533300218</v>
+        <v>-0.60654829630578966</v>
       </c>
       <c r="F10">
-        <v>5.9980780022719817E-2</v>
+        <v>9.8272571977688836E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -612,19 +612,19 @@
         <v>25000</v>
       </c>
       <c r="B11">
-        <v>-7.4014254941662624E-2</v>
+        <v>-0.4567869402832444</v>
       </c>
       <c r="C11">
-        <v>3.9866399379151964E-2</v>
+        <v>0.13201487556311672</v>
       </c>
       <c r="D11">
         <v>25000</v>
       </c>
       <c r="E11">
-        <v>-0.37295763024849116</v>
+        <v>-0.52432440156333826</v>
       </c>
       <c r="F11">
-        <v>0.18812529855884938</v>
+        <v>8.3679854746235474E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -632,19 +632,19 @@
         <v>50000</v>
       </c>
       <c r="B12">
-        <v>9.904670153222514E-2</v>
+        <v>-0.46705563274573852</v>
       </c>
       <c r="C12">
-        <v>0.21619630652660923</v>
+        <v>0.19790993866410758</v>
       </c>
       <c r="D12">
         <v>50000</v>
       </c>
       <c r="E12">
-        <v>-0.33685746001731887</v>
+        <v>-0.50194259505310856</v>
       </c>
       <c r="F12">
-        <v>0.39711874162784655</v>
+        <v>8.7700262946413907E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,19 +652,19 @@
         <v>75000</v>
       </c>
       <c r="B13">
-        <v>4.0977825695269102E-2</v>
+        <v>-0.31640141691248291</v>
       </c>
       <c r="C13">
-        <v>0.1910577524625181</v>
+        <v>0.15260802853115521</v>
       </c>
       <c r="D13">
         <v>75000</v>
       </c>
       <c r="E13">
-        <v>-0.17277398633083296</v>
+        <v>-0.37094760173824454</v>
       </c>
       <c r="F13">
-        <v>0.32179638048913772</v>
+        <v>3.4213289602273357E-2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -672,19 +672,19 @@
         <v>100000</v>
       </c>
       <c r="B14">
-        <v>-3.0238068212590161E-2</v>
+        <v>-0.19606272965002822</v>
       </c>
       <c r="C14">
-        <v>0.16068318134371706</v>
+        <v>0.15188659547920363</v>
       </c>
       <c r="D14">
         <v>100000</v>
       </c>
       <c r="E14">
-        <v>5.5662791659223755E-2</v>
+        <v>-0.2918889387452322</v>
       </c>
       <c r="F14">
-        <v>0.32993065923658454</v>
+        <v>5.7811742319382908E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -692,19 +692,19 @@
         <v>250000</v>
       </c>
       <c r="B15">
-        <v>0.42836367397691621</v>
+        <v>0.1299361964062403</v>
       </c>
       <c r="C15">
-        <v>0.11191198215485958</v>
+        <v>0.16033818244642659</v>
       </c>
       <c r="D15">
         <v>250000</v>
       </c>
       <c r="E15">
-        <v>0.38514592428454408</v>
+        <v>0.11782719851896012</v>
       </c>
       <c r="F15">
-        <v>0.12001081472740294</v>
+        <v>8.5837622021543047E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -712,19 +712,19 @@
         <v>500000</v>
       </c>
       <c r="B16">
-        <v>0.56586719192782686</v>
+        <v>0.16475072365605853</v>
       </c>
       <c r="C16">
-        <v>1.0959460533742194E-2</v>
+        <v>0.13599792518712098</v>
       </c>
       <c r="D16">
         <v>500000</v>
       </c>
       <c r="E16">
-        <v>0.59146704527658767</v>
+        <v>0.22188292652923658</v>
       </c>
       <c r="F16">
-        <v>0.20916905713540757</v>
+        <v>5.7338832850483613E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -732,19 +732,19 @@
         <v>750000</v>
       </c>
       <c r="B17">
-        <v>0.66713687592446858</v>
+        <v>0.19917717017401507</v>
       </c>
       <c r="C17">
-        <v>2.3477222488404337E-2</v>
+        <v>0.12224362027973096</v>
       </c>
       <c r="D17">
         <v>750000</v>
       </c>
       <c r="E17">
-        <v>0.77638440889489313</v>
+        <v>0.31150046430200851</v>
       </c>
       <c r="F17">
-        <v>7.7138400123631143E-2</v>
+        <v>0.1178292920692353</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -752,19 +752,19 @@
         <v>1000000</v>
       </c>
       <c r="B18">
-        <v>0.50456046458947545</v>
+        <v>0.220766627065586</v>
       </c>
       <c r="C18">
-        <v>7.9843213429686616E-2</v>
+        <v>0.11804956101628347</v>
       </c>
       <c r="D18">
         <v>1000000</v>
       </c>
       <c r="E18">
-        <v>0.7580928399040161</v>
+        <v>0.29317027561130621</v>
       </c>
       <c r="F18">
-        <v>0.13261840287987545</v>
+        <v>3.9482946632506004E-2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -772,19 +772,19 @@
         <v>2500000</v>
       </c>
       <c r="B19">
-        <v>0.6820989973803806</v>
+        <v>0.28213767852434346</v>
       </c>
       <c r="C19">
-        <v>0.50508268960410541</v>
+        <v>0.13520794830215169</v>
       </c>
       <c r="D19">
         <v>2500000</v>
       </c>
       <c r="E19">
-        <v>0.66294164016654455</v>
+        <v>0.37906832448184824</v>
       </c>
       <c r="F19">
-        <v>0.1179046349504948</v>
+        <v>3.2387768761737781E-2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,19 +792,19 @@
         <v>5000000</v>
       </c>
       <c r="B20">
-        <v>0.89107337444981338</v>
+        <v>0.27314833850634956</v>
       </c>
       <c r="C20">
-        <v>2.6356633428197773E-2</v>
+        <v>0.14440452734196738</v>
       </c>
       <c r="D20">
         <v>5000000</v>
       </c>
       <c r="E20">
-        <v>0.81233222359434565</v>
+        <v>0.3187644442774431</v>
       </c>
       <c r="F20">
-        <v>0.1440227386734568</v>
+        <v>6.3071113126602379E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -812,19 +812,19 @@
         <v>7500000</v>
       </c>
       <c r="B21">
-        <v>0.910300606328446</v>
+        <v>0.36483271021810537</v>
       </c>
       <c r="C21">
-        <v>7.1252179468781318E-2</v>
+        <v>0.33126737937098399</v>
       </c>
       <c r="D21">
         <v>7500000</v>
       </c>
       <c r="E21">
-        <v>0.63781713526729467</v>
+        <v>0.31712292811763992</v>
       </c>
       <c r="F21">
-        <v>0.22481127137781445</v>
+        <v>7.3621514553064843E-3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,19 +832,19 @@
         <v>10000000</v>
       </c>
       <c r="B22">
-        <v>0.90298415041241431</v>
+        <v>0.33230113139332407</v>
       </c>
       <c r="C22">
-        <v>6.3392517323690445E-4</v>
+        <v>0.31266274071808814</v>
       </c>
       <c r="D22">
         <v>10000000</v>
       </c>
       <c r="E22">
-        <v>0.78425164557443505</v>
+        <v>0.39168198863066528</v>
       </c>
       <c r="F22">
-        <v>4.3977993323935663E-2</v>
+        <v>0.11487933279312987</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -852,19 +852,19 @@
         <v>25000000</v>
       </c>
       <c r="B23">
-        <v>0.75761336699998583</v>
+        <v>0.22899164498772792</v>
       </c>
       <c r="C23">
-        <v>8.6108828289424566E-3</v>
+        <v>0.16559437662319845</v>
       </c>
       <c r="D23">
         <v>25000000</v>
       </c>
       <c r="E23">
-        <v>0.55015494283825517</v>
+        <v>0.28189854046039264</v>
       </c>
       <c r="F23">
-        <v>0.20988212077332605</v>
+        <v>2.6527228202338365E-2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -872,19 +872,19 @@
         <v>50000000</v>
       </c>
       <c r="B24">
-        <v>0.21421565646347068</v>
+        <v>8.8689891187378772E-2</v>
       </c>
       <c r="C24">
-        <v>0.24106062441463083</v>
+        <v>0.1250286374618241</v>
       </c>
       <c r="D24">
         <v>50000000</v>
       </c>
       <c r="E24">
-        <v>0.37117113066183743</v>
+        <v>2.5903360038669384E-2</v>
       </c>
       <c r="F24">
-        <v>8.2982307625799154E-2</v>
+        <v>3.4911251773242793E-2</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,13 +916,13 @@
         <v>3500</v>
       </c>
       <c r="B28" s="1">
-        <v>-0.49600351946847288</v>
+        <v>-0.4974538692281173</v>
       </c>
       <c r="D28">
         <v>3500</v>
       </c>
       <c r="E28">
-        <v>-0.34392229588162909</v>
+        <v>-0.49747933569959207</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -930,13 +930,13 @@
         <v>4289.983887686757</v>
       </c>
       <c r="B29">
-        <v>-0.49509421131100478</v>
+        <v>-0.49726031873780269</v>
       </c>
       <c r="D29">
         <v>4289.983887686757</v>
       </c>
       <c r="E29">
-        <v>-0.3436725073977509</v>
+        <v>-0.49735028192046599</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,13 +944,13 @@
         <v>5258.2747876034291</v>
       </c>
       <c r="B30">
-        <v>-0.49373049900064309</v>
+        <v>-0.49696969762550341</v>
       </c>
       <c r="D30">
         <v>5258.2747876034291</v>
       </c>
       <c r="E30">
-        <v>-0.34329744067949219</v>
+        <v>-0.49715646269806157</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -958,13 +958,13 @@
         <v>6445.1183188137757</v>
       </c>
       <c r="B31">
-        <v>-0.49168710478193078</v>
+        <v>-0.49653344462173499</v>
       </c>
       <c r="D31">
         <v>6445.1183188137757</v>
       </c>
       <c r="E31">
-        <v>-0.34273441960689738</v>
+        <v>-0.49686542576313147</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -972,13 +972,13 @@
         <v>7899.8439262702441</v>
       </c>
       <c r="B32">
-        <v>-0.48862930614169769</v>
+        <v>-0.49587885795414521</v>
       </c>
       <c r="D32">
         <v>7899.8439262702441</v>
       </c>
       <c r="E32">
-        <v>-0.34188960647455491</v>
+        <v>-0.49642852081208078</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -986,13 +986,13 @@
         <v>9682.91518826842</v>
       </c>
       <c r="B33">
-        <v>-0.48406253849761</v>
+        <v>-0.49489728630488927</v>
       </c>
       <c r="D33">
         <v>9682.91518826842</v>
       </c>
       <c r="E33">
-        <v>-0.34062275287963029</v>
+        <v>-0.49577289341086928</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,13 +1000,13 @@
         <v>11868.4428981454</v>
       </c>
       <c r="B34">
-        <v>-0.47726220647856621</v>
+        <v>-0.49342678220891217</v>
       </c>
       <c r="D34">
         <v>11868.4428981454</v>
       </c>
       <c r="E34">
-        <v>-0.33872479299682628</v>
+        <v>-0.49478962054685682</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1014,13 +1014,13 @@
         <v>14547.26537284975</v>
       </c>
       <c r="B35">
-        <v>-0.46718016701897769</v>
+        <v>-0.49122692008047009</v>
       </c>
       <c r="D35">
         <v>14547.26537284975</v>
       </c>
       <c r="E35">
-        <v>-0.33588530030975761</v>
+        <v>-0.49331625207152552</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1028,13 +1028,13 @@
         <v>17830.724016979679</v>
       </c>
       <c r="B36">
-        <v>-0.45232941653288411</v>
+        <v>-0.48794290635566351</v>
       </c>
       <c r="D36">
         <v>17830.724016979679</v>
       </c>
       <c r="E36">
-        <v>-0.33164607143533009</v>
+        <v>-0.49111139747748461</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1042,13 +1042,13 @@
         <v>21855.291068180621</v>
       </c>
       <c r="B37">
-        <v>-0.43066218260327338</v>
+        <v>-0.48305590805362542</v>
       </c>
       <c r="D37">
         <v>21855.291068180621</v>
       </c>
       <c r="E37">
-        <v>-0.32533680825528272</v>
+        <v>-0.48781835215361508</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,13 +1056,13 @@
         <v>26788.241869485501</v>
       </c>
       <c r="B38">
-        <v>-0.39948590595860151</v>
+        <v>-0.47581756981488688</v>
       </c>
       <c r="D38">
         <v>26788.241869485501</v>
       </c>
       <c r="E38">
-        <v>-0.31599015144034381</v>
+        <v>-0.4829144101133554</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,13 +1070,13 @@
         <v>32834.60742844241</v>
       </c>
       <c r="B39">
-        <v>-0.35551264128964433</v>
+        <v>-0.46517083033188422</v>
       </c>
       <c r="D39">
         <v>32834.60742844241</v>
       </c>
       <c r="E39">
-        <v>-0.30223854270298012</v>
+        <v>-0.47564326460728501</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1084,13 +1084,13 @@
         <v>40245.696236153708</v>
       </c>
       <c r="B40">
-        <v>-0.29520212706980142</v>
+        <v>-0.44966978068152352</v>
       </c>
       <c r="D40">
         <v>40245.696236153708</v>
       </c>
       <c r="E40">
-        <v>-0.28220892359613747</v>
+        <v>-0.46493150616579992</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1098,13 +1098,13 @@
         <v>49329.53954338147</v>
       </c>
       <c r="B41">
-        <v>-0.21558532358799329</v>
+        <v>-0.42743330920513262</v>
       </c>
       <c r="D41">
         <v>49329.53954338147</v>
       </c>
       <c r="E41">
-        <v>-0.25345946143290848</v>
+        <v>-0.44930000616529803</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1112,13 +1112,13 @@
         <v>60463.694236603849</v>
       </c>
       <c r="B42">
-        <v>-0.11562136168614361</v>
+        <v>-0.39620401443951542</v>
       </c>
       <c r="D42">
         <v>60463.694236603849</v>
       </c>
       <c r="E42">
-        <v>-0.21304993991724261</v>
+        <v>-0.42680199673186081</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1126,13 +1126,13 @@
         <v>74110.935447156822</v>
       </c>
       <c r="B43">
-        <v>2.279115916142084E-3</v>
+        <v>-0.3536264813035826</v>
       </c>
       <c r="D43">
         <v>74110.935447156822</v>
       </c>
       <c r="E43">
-        <v>-0.15789348386259111</v>
+        <v>-0.39505644685248398</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,13 +1140,13 @@
         <v>90838.491134198979</v>
       </c>
       <c r="B44">
-        <v>0.13149659200951649</v>
+        <v>-0.29786507358710451</v>
       </c>
       <c r="D44">
         <v>90838.491134198979</v>
       </c>
       <c r="E44">
-        <v>-8.5548342536546307E-2</v>
+        <v>-0.35149235080277602</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,13 +1154,13 @@
         <v>111341.6180992827</v>
       </c>
       <c r="B45">
-        <v>0.26221023812292749</v>
+        <v>-0.22856202817515439</v>
       </c>
       <c r="D45">
         <v>111341.6180992827</v>
       </c>
       <c r="E45">
-        <v>4.5401512395951754E-3</v>
+        <v>-0.29393991222527288</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1168,13 +1168,13 @@
         <v>136472.49933568441</v>
       </c>
       <c r="B46">
-        <v>0.38414479651821209</v>
+        <v>-0.14782215136835319</v>
       </c>
       <c r="D46">
         <v>136472.49933568441</v>
       </c>
       <c r="E46">
-        <v>0.1097409270377912</v>
+        <v>-0.22161038078195641</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1182,13 +1182,13 @@
         <v>167275.66378926529</v>
       </c>
       <c r="B47">
-        <v>0.48958685273044378</v>
+        <v>-6.0550811277864172E-2</v>
       </c>
       <c r="D47">
         <v>167275.66378926529</v>
       </c>
       <c r="E47">
-        <v>0.22375185593731789</v>
+        <v>-0.13620502274147669</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1196,13 +1196,13 @@
         <v>205031.4007023017</v>
       </c>
       <c r="B48">
-        <v>0.57495348527914081</v>
+        <v>2.645800530178621E-2</v>
       </c>
       <c r="D48">
         <v>205031.4007023017</v>
       </c>
       <c r="E48">
-        <v>0.33773541153093878</v>
+        <v>-4.2482017775671482E-2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1210,13 +1210,13 @@
         <v>251308.972995063</v>
       </c>
       <c r="B49">
-        <v>0.64045434007461377</v>
+        <v>0.10648610026340941</v>
       </c>
       <c r="D49">
         <v>251308.972995063</v>
       </c>
       <c r="E49">
-        <v>0.44286172879412278</v>
+        <v>5.2449574406654077E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1224,13 +1224,13 @@
         <v>308031.84142283653</v>
       </c>
       <c r="B50">
-        <v>0.68867018533132152</v>
+        <v>0.17480939847979049</v>
       </c>
       <c r="D50">
         <v>308031.84142283653</v>
       </c>
       <c r="E50">
-        <v>0.53284693596354959</v>
+        <v>0.14110868211513411</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1238,13 +1238,13 @@
         <v>377557.6104566998</v>
       </c>
       <c r="B51">
-        <v>0.72308646328652104</v>
+        <v>0.22951372726726799</v>
       </c>
       <c r="D51">
         <v>377557.6104566998</v>
       </c>
       <c r="E51">
-        <v>0.60507893343950403</v>
+        <v>0.21784018673067501</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,13 +1252,13 @@
         <v>462776.01872364478</v>
       </c>
       <c r="B52">
-        <v>0.74711214383285218</v>
+        <v>0.27108420046751691</v>
       </c>
       <c r="D52">
         <v>462776.01872364478</v>
       </c>
       <c r="E52">
-        <v>0.66012455788128988</v>
+        <v>0.27997704280164482</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1266,13 +1266,13 @@
         <v>567229.04683778947</v>
       </c>
       <c r="B53">
-        <v>0.76361825172074227</v>
+        <v>0.30140103922892142</v>
       </c>
       <c r="D53">
         <v>567229.04683778947</v>
       </c>
       <c r="E53">
-        <v>0.70042879128538948</v>
+        <v>0.3276134148133929</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,13 +1280,13 @@
         <v>695258.13473201031</v>
       </c>
       <c r="B54">
-        <v>0.77482390713192417</v>
+        <v>0.32279663311212992</v>
       </c>
       <c r="D54">
         <v>695258.13473201031</v>
       </c>
       <c r="E54">
-        <v>0.72907412452534415</v>
+        <v>0.36257602583812831</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1294,13 +1294,13 @@
         <v>852184.62736670556</v>
       </c>
       <c r="B55">
-        <v>0.78235424683903998</v>
+        <v>0.33745922818187302</v>
       </c>
       <c r="D55">
         <v>852184.62736670556</v>
       </c>
       <c r="E55">
-        <v>0.74899061921595411</v>
+        <v>0.38735081676333782</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1308,13 +1308,13 @@
         <v>1044530.948782147</v>
       </c>
       <c r="B56">
-        <v>0.78735657863671027</v>
+        <v>0.3471668517854094</v>
       </c>
       <c r="D56">
         <v>1044530.948782147</v>
       </c>
       <c r="E56">
-        <v>0.76260488891907563</v>
+        <v>0.40435676699458439</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1322,13 +1322,13 @@
         <v>1280291.6972758761</v>
       </c>
       <c r="B57">
-        <v>0.79061797115974697</v>
+        <v>0.35322772717739143</v>
       </c>
       <c r="D57">
         <v>1280291.6972758761</v>
       </c>
       <c r="E57">
-        <v>0.77176880063169595</v>
+        <v>0.41559532400743049</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1336,13 +1336,13 @@
         <v>1569265.92938647</v>
       </c>
       <c r="B58">
-        <v>0.79266241022283856</v>
+        <v>0.35651417376860639</v>
       </c>
       <c r="D58">
         <v>1569265.92938647</v>
       </c>
       <c r="E58">
-        <v>0.77782016190111769</v>
+        <v>0.42255006360289082</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1350,13 +1350,13 @@
         <v>1923464.4435896419</v>
       </c>
       <c r="B59">
-        <v>0.79382277605501228</v>
+        <v>0.35751967610533342</v>
       </c>
       <c r="D59">
         <v>1923464.4435896419</v>
       </c>
       <c r="E59">
-        <v>0.78168357554821566</v>
+        <v>0.42620666030389781</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1364,13 +1364,13 @@
         <v>2357608.9918679842</v>
       </c>
       <c r="B60">
-        <v>0.79428957585647608</v>
+        <v>0.35640443114536441</v>
       </c>
       <c r="D60">
         <v>2357608.9918679842</v>
       </c>
       <c r="E60">
-        <v>0.78396675584489184</v>
+        <v>0.42710769795409209</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,13 +1378,13 @@
         <v>2889744.1681654458</v>
       </c>
       <c r="B61">
-        <v>0.79413991406230067</v>
+        <v>0.35301645552468669</v>
       </c>
       <c r="D61">
         <v>2889744.1681654458</v>
       </c>
       <c r="E61">
-        <v>0.78503535217180109</v>
+        <v>0.42539853600982341</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,13 +1392,13 @@
         <v>3541987.4059904418</v>
       </c>
       <c r="B62">
-        <v>0.79334954062686014</v>
+        <v>0.34688820581020352</v>
       </c>
       <c r="D62">
         <v>3541987.4059904418</v>
       </c>
       <c r="E62">
-        <v>0.78506233893746924</v>
+        <v>0.42084761834530487</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1406,13 +1406,13 @@
         <v>4341448.2577395402</v>
       </c>
       <c r="B63">
-        <v>0.79178938986129921</v>
+        <v>0.33721972339477352</v>
       </c>
       <c r="D63">
         <v>4341448.2577395402</v>
       </c>
       <c r="E63">
-        <v>0.78405263143409154</v>
+        <v>0.41284192219272059</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1420,13 +1420,13 @@
         <v>5321355.1642652536</v>
       </c>
       <c r="B64">
-        <v>0.78920643893678266</v>
+        <v>0.32287503946718099</v>
       </c>
       <c r="D64">
         <v>5321355.1642652536</v>
       </c>
       <c r="E64">
-        <v>0.78184416833662829</v>
+        <v>0.40037407086862381</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1434,13 +1434,13 @@
         <v>6522436.5472447649</v>
       </c>
       <c r="B65">
-        <v>0.78518736073502116</v>
+        <v>0.30244274413524003</v>
       </c>
       <c r="D65">
         <v>6522436.5472447649</v>
       </c>
       <c r="E65">
-        <v>0.77808580512979297</v>
+        <v>0.38205951829937562</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1448,13 +1448,13 @@
         <v>7994613.6274683746</v>
       </c>
       <c r="B66">
-        <v>0.77910287693849767</v>
+        <v>0.27443855095314101</v>
       </c>
       <c r="D66">
         <v>7994613.6274683746</v>
       </c>
       <c r="E66">
-        <v>0.77219161043603746</v>
+        <v>0.35625262299526461</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1462,13 +1462,13 @@
         <v>9799075.3286057916</v>
       </c>
       <c r="B67">
-        <v>0.77003213375681268</v>
+        <v>0.23772850666551379</v>
       </c>
       <c r="D67">
         <v>9799075.3286057916</v>
       </c>
       <c r="E67">
-        <v>0.76327221452580696</v>
+        <v>0.32135619165259721</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1476,13 +1476,13 @@
         <v>12010821.5068422</v>
       </c>
       <c r="B68">
-        <v>0.75667229609117492</v>
+        <v>0.19216722706417469</v>
       </c>
       <c r="D68">
         <v>12010821.5068422</v>
       </c>
       <c r="E68">
-        <v>0.75004936964980351</v>
+        <v>0.27639521588338212</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1490,13 +1490,13 @@
         <v>14721780.212067019</v>
       </c>
       <c r="B69">
-        <v>0.73725323411973531</v>
+        <v>0.1392342550652397</v>
       </c>
       <c r="D69">
         <v>14721780.212067019</v>
       </c>
       <c r="E69">
-        <v>0.73077422762856337</v>
+        <v>0.22178093675883229</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,13 +1504,13 @@
         <v>18044628.545095231</v>
       </c>
       <c r="B70">
-        <v>0.70950633090989967</v>
+        <v>8.2222287233497615E-2</v>
       </c>
       <c r="D70">
         <v>18044628.545095231</v>
       </c>
       <c r="E70">
-        <v>0.70319866218321914</v>
+        <v>0.15991801331903729</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,13 +1518,13 @@
         <v>22117475.919357471</v>
       </c>
       <c r="B71">
-        <v>0.67078201295959483</v>
+        <v>2.559962003103914E-2</v>
       </c>
       <c r="D71">
         <v>22117475.919357471</v>
       </c>
       <c r="E71">
-        <v>0.66469414766650115</v>
+        <v>9.5119614569177335E-2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1532,13 +1532,13 @@
         <v>27109604.380098131</v>
       </c>
       <c r="B72">
-        <v>0.61845541312233765</v>
+        <v>-2.6289545614991031E-2</v>
       </c>
       <c r="D72">
         <v>27109604.380098131</v>
       </c>
       <c r="E72">
-        <v>0.61265705004542148</v>
+        <v>3.2565457335056128E-2</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1546,13 +1546,13 @@
         <v>33228504.5691952</v>
       </c>
       <c r="B73">
-        <v>0.55074141112584152</v>
+        <v>-7.0452736368635832E-2</v>
       </c>
       <c r="D73">
         <v>33228504.5691952</v>
       </c>
       <c r="E73">
-        <v>0.54532066300626869</v>
+        <v>-2.32465807816499E-2</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1560,13 +1560,13 @@
         <v>40728499.77536381</v>
       </c>
       <c r="B74">
-        <v>0.46784997122606581</v>
+        <v>-0.1057370974883803</v>
       </c>
       <c r="D74">
         <v>40728499.77536381</v>
       </c>
       <c r="E74">
-        <v>0.46290435182413581</v>
+        <v>-6.9650898411762446E-2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1574,13 +1574,13 @@
         <v>49921316.5159899</v>
       </c>
       <c r="B75">
-        <v>0.37300796128392422</v>
+        <v>-0.1325305848521712</v>
       </c>
       <c r="D75">
         <v>49921316.5159899</v>
       </c>
       <c r="E75">
-        <v>0.36862740376563902</v>
+        <v>-0.1060232282231329</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1588,13 +1588,13 @@
         <v>61189041.001630627</v>
       </c>
       <c r="B76">
-        <v>0.27252647926791701</v>
+        <v>-0.1521016073912437</v>
       </c>
       <c r="D76">
         <v>61189041.001630627</v>
       </c>
       <c r="E76">
-        <v>0.26877135584208628</v>
+        <v>-0.13323651582667731</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1602,13 +1602,13 @@
         <v>75000000.000000015</v>
       </c>
       <c r="B77" s="2">
-        <v>0.17438328861527111</v>
+        <v>-0.16599528552081569</v>
       </c>
       <c r="D77">
         <v>75000000.000000015</v>
       </c>
       <c r="E77" s="2">
-        <v>0.17126638413300169</v>
+        <v>-0.15289676475793579</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>